<commit_message>
Separate DeviceConfig from appConfig, Modify method in Lxsetup.class, Change Key in scripts.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/100.30.10_InstallandUninstallprocess.xlsx
+++ b/NformTester/NformTester/Keywordscripts/100.30.10_InstallandUninstallprocess.xlsx
@@ -3713,10 +3713,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$SNMP_GXT_0$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"Description for GXT"</t>
   </si>
   <si>
@@ -3859,6 +3855,9 @@
   <si>
     <t>ButtonIgnore</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$NAME_SNMP_GXT_0$</t>
   </si>
 </sst>
 </file>
@@ -4896,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4965,7 +4964,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="15"/>
@@ -4996,7 +4995,7 @@
         <v>809</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -5019,7 +5018,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -5129,7 +5128,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>794</v>
@@ -5936,7 +5935,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="15"/>
@@ -5973,16 +5972,16 @@
         <v>819</v>
       </c>
       <c r="J38" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="L38" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="M38" s="4" t="s">
         <v>822</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>823</v>
       </c>
       <c r="N38" s="13"/>
       <c r="O38" s="12"/>
@@ -5994,7 +5993,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -6105,7 +6104,7 @@
         <v>4</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
@@ -6133,7 +6132,7 @@
         <v>4</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
@@ -6239,7 +6238,7 @@
         <v>4</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="I48" s="22"/>
       <c r="J48" s="22"/>
@@ -6267,7 +6266,7 @@
         <v>4</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="I49" s="22"/>
       <c r="J49" s="22"/>
@@ -6295,7 +6294,7 @@
         <v>4</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
@@ -6321,7 +6320,7 @@
         <v>4</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
@@ -6410,7 +6409,7 @@
         <v>805</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F55" s="22">
         <v>2</v>
@@ -6429,7 +6428,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="22"/>
@@ -6495,23 +6494,23 @@
         <v>58</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="22" t="s">
+        <v>834</v>
+      </c>
+      <c r="I59" s="22" t="s">
         <v>835</v>
       </c>
-      <c r="I59" s="22" t="s">
+      <c r="J59" s="22" t="s">
         <v>836</v>
-      </c>
-      <c r="J59" s="22" t="s">
-        <v>837</v>
       </c>
       <c r="K59" s="22"/>
       <c r="L59" s="22"/>
@@ -6583,7 +6582,7 @@
         <v>56</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I62" s="22"/>
       <c r="J62" s="22"/>
@@ -6645,7 +6644,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="4"/>
@@ -6664,17 +6663,17 @@
         <v>65</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E66" s="22" t="s">
         <v>572</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I66" s="22"/>
       <c r="J66" s="22"/>
@@ -6742,7 +6741,7 @@
         <v>805</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F69" s="15">
         <v>5</v>
@@ -6762,7 +6761,7 @@
         <v>69</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="15"/>
@@ -6804,10 +6803,10 @@
         <v>71</v>
       </c>
       <c r="D72" s="14" t="s">
+        <v>845</v>
+      </c>
+      <c r="E72" s="15" t="s">
         <v>846</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>847</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>669</v>
@@ -6829,13 +6828,13 @@
         <v>72</v>
       </c>
       <c r="D73" s="14" t="s">
+        <v>845</v>
+      </c>
+      <c r="E73" s="15" t="s">
         <v>846</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="F73" s="15" t="s">
         <v>847</v>
-      </c>
-      <c r="F73" s="15" t="s">
-        <v>848</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>2</v>
@@ -6854,7 +6853,7 @@
         <v>73</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E74" s="15" t="s">
         <v>680</v>
@@ -6879,10 +6878,10 @@
         <v>74</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F75" s="15" t="s">
         <v>683</v>
@@ -6904,13 +6903,13 @@
         <v>75</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E76" s="15" t="s">
+        <v>856</v>
+      </c>
+      <c r="F76" s="15" t="s">
         <v>857</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>858</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>2</v>
@@ -6929,10 +6928,10 @@
         <v>76</v>
       </c>
       <c r="D77" s="14" t="s">
+        <v>843</v>
+      </c>
+      <c r="E77" s="15" t="s">
         <v>844</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>845</v>
       </c>
       <c r="F77" s="15">
         <v>30</v>
@@ -6954,10 +6953,10 @@
         <v>786</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G78" s="15" t="s">
         <v>2</v>
@@ -6978,7 +6977,7 @@
         <v>805</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F79" s="15">
         <v>5</v>
@@ -6997,7 +6996,7 @@
         <v>79</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
@@ -7021,7 +7020,7 @@
         <v>809</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="15"/>
@@ -8940,7 +8939,7 @@
         <v>666</v>
       </c>
       <c r="BO12" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="BP12" t="s">
         <v>583</v>

</xml_diff>